<commit_message>
Zero'd and History deleted
</commit_message>
<xml_diff>
--- a/ProductionBudgetSheetWatch.xlsx
+++ b/ProductionBudgetSheetWatch.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\DGM_1660\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88E60E93-C3AA-487A-B909-4EA62D0E0D59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A0B4B6-36C6-4D0F-8F62-2151D555D411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="115">
   <si>
     <t>Model To Animate</t>
   </si>
@@ -402,6 +402,12 @@
   </si>
   <si>
     <t>WatchBuckle</t>
+  </si>
+  <si>
+    <t>WatchBuckle Miscellanious Pieces</t>
+  </si>
+  <si>
+    <t>WatchBody Edits</t>
   </si>
 </sst>
 </file>
@@ -968,8 +974,8 @@
   </sheetPr>
   <dimension ref="A1:Z52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1497,7 +1503,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="7">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -1506,9 +1512,15 @@
       <c r="H32" s="11"/>
     </row>
     <row r="33" spans="1:8" ht="12.75">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
+      <c r="A33" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" s="7">
+        <v>30</v>
+      </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -1516,9 +1528,15 @@
       <c r="H33" s="11"/>
     </row>
     <row r="34" spans="1:8" ht="12.75">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
+      <c r="A34" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="7">
+        <v>10</v>
+      </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>

</xml_diff>

<commit_message>
Time Budget Sheet updated and Final(?) UV Mapping Complete
</commit_message>
<xml_diff>
--- a/ProductionBudgetSheetWatch.xlsx
+++ b/ProductionBudgetSheetWatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\School\DGM_1660\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A0B4B6-36C6-4D0F-8F62-2151D555D411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{61151AAA-C206-478E-9DB2-47F0348B4192}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -857,7 +857,7 @@
       </c>
       <c r="B4" s="13">
         <f>TotalModelTime</f>
-        <v>53.5</v>
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="12.75">
@@ -911,7 +911,7 @@
       </c>
       <c r="B10" s="23">
         <f>SUM(B4:B9)</f>
-        <v>155.1</v>
+        <v>417.6</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -975,7 +975,7 @@
   <dimension ref="A1:Z52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1409,11 +1409,16 @@
       <c r="C26" s="7">
         <v>3</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="7">
+        <v>10</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="11"/>
+      <c r="H26" s="11">
+        <f>SUM(C26:G26)</f>
+        <v>13</v>
+      </c>
     </row>
     <row r="27" spans="1:11" ht="12.75">
       <c r="A27" s="7" t="s">
@@ -1429,7 +1434,10 @@
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="11"/>
+      <c r="H27" s="11">
+        <f>SUM(C27:G27)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="1:11" ht="12.75">
       <c r="A28" s="7" t="s">
@@ -1445,7 +1453,9 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="11"/>
+      <c r="H28" s="11">
+        <v>4</v>
+      </c>
     </row>
     <row r="29" spans="1:11" ht="12.75">
       <c r="A29" s="7" t="s">
@@ -1457,11 +1467,16 @@
       <c r="C29" s="7">
         <v>0.5</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="11"/>
+      <c r="H29" s="11">
+        <f>SUM(C29:D29)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:11" ht="12.75">
       <c r="A30" s="7" t="s">
@@ -1473,11 +1488,16 @@
       <c r="C30" s="7">
         <v>2</v>
       </c>
-      <c r="D30" s="7"/>
+      <c r="D30" s="7">
+        <v>0.5</v>
+      </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="11"/>
+      <c r="H30" s="11">
+        <f>SUM(C30:D30)</f>
+        <v>2.5</v>
+      </c>
     </row>
     <row r="31" spans="1:11" ht="12.75">
       <c r="A31" s="7" t="s">
@@ -1489,11 +1509,16 @@
       <c r="C31" s="7">
         <v>20</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="7">
+        <v>120</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="11"/>
+      <c r="H31" s="11">
+        <f>SUM(C31:E31)</f>
+        <v>140</v>
+      </c>
     </row>
     <row r="32" spans="1:11" ht="12.75">
       <c r="A32" s="7" t="s">
@@ -1505,11 +1530,16 @@
       <c r="C32" s="7">
         <v>20</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="7">
+        <v>30</v>
+      </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-      <c r="H32" s="11"/>
+      <c r="H32" s="11">
+        <f>SUM(C32:D32)</f>
+        <v>50</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="12.75">
       <c r="A33" s="7" t="s">
@@ -1521,11 +1551,16 @@
       <c r="C33" s="7">
         <v>30</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="7">
+        <v>10</v>
+      </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="11"/>
+      <c r="H33" s="11">
+        <f>SUM(C33:D33)</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="12.75">
       <c r="A34" s="7" t="s">
@@ -1541,7 +1576,9 @@
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-      <c r="H34" s="11"/>
+      <c r="H34" s="11">
+        <v>10</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="12.75">
       <c r="A35" s="7"/>
@@ -1709,7 +1746,7 @@
       </c>
       <c r="H51" s="16">
         <f>SUM(H26:H50)</f>
-        <v>0</v>
+        <v>262.5</v>
       </c>
       <c r="J51" s="21"/>
       <c r="K51" s="21"/>
@@ -1720,7 +1757,7 @@
       </c>
       <c r="H52" s="20">
         <f>SUM(H7, H24, H51)</f>
-        <v>53.5</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>